<commit_message>
issues 9 and 10 still pending
</commit_message>
<xml_diff>
--- a/scrum.xlsx
+++ b/scrum.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ebeth_000\Documents\marc\music_app\"/>
@@ -14,17 +14,20 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>date</t>
   </si>
@@ -69,6 +72,9 @@
   </si>
   <si>
     <t>Allow notes to change while playing loop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chords should be an octave lowerr than the melody </t>
   </si>
 </sst>
 </file>
@@ -84,7 +90,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -103,6 +109,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -116,11 +128,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -181,7 +194,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -233,7 +246,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -435,13 +448,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="63.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -551,8 +564,24 @@
         <v>7</v>
       </c>
     </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>42599</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Resolved issues 7 and 10
</commit_message>
<xml_diff>
--- a/scrum.xlsx
+++ b/scrum.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>date</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t xml:space="preserve">chords should be an octave lowerr than the melody </t>
+  </si>
+  <si>
+    <t>last and secondLast classes not playing notes</t>
   </si>
 </sst>
 </file>
@@ -194,7 +197,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -246,7 +249,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -448,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,7 +542,7 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -572,6 +575,17 @@
         <v>15</v>
       </c>
       <c r="C10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>42602</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
columns no longer depended on starting key
</commit_message>
<xml_diff>
--- a/scrum.xlsx
+++ b/scrum.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>date</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>clean up the keyboard</t>
+  </si>
+  <si>
+    <t>draft58</t>
   </si>
 </sst>
 </file>
@@ -460,7 +463,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,7 +565,10 @@
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
issues discussed 8/22. Loop not working
</commit_message>
<xml_diff>
--- a/scrum.xlsx
+++ b/scrum.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
   <si>
     <t>date</t>
   </si>
@@ -87,6 +87,27 @@
   </si>
   <si>
     <t>draft58</t>
+  </si>
+  <si>
+    <t>Piano keys should change the column</t>
+  </si>
+  <si>
+    <t>Split black piano keys into sharp and flat</t>
+  </si>
+  <si>
+    <t>could use labels</t>
+  </si>
+  <si>
+    <t>Bassline should be the bottom of each chord</t>
+  </si>
+  <si>
+    <t>notes need to change for top 2 rows</t>
+  </si>
+  <si>
+    <t>Remove low-register buttons</t>
+  </si>
+  <si>
+    <t>Remove sharps and flats during calibration</t>
   </si>
 </sst>
 </file>
@@ -102,7 +123,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -127,6 +148,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -140,12 +167,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,6 +643,75 @@
         <v>7</v>
       </c>
     </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>42604</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>42604</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>42604</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>42604</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>42604</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>42604</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
cols on the ends can play
</commit_message>
<xml_diff>
--- a/scrum.xlsx
+++ b/scrum.xlsx
@@ -62,9 +62,6 @@
     <t>mp3 not playing or not simultaneous</t>
   </si>
   <si>
-    <t>possible browser compatibility issue. Will adjust duration of mp3 playback</t>
-  </si>
-  <si>
     <t>clone chords above melody to mark below melody</t>
   </si>
   <si>
@@ -108,6 +105,9 @@
   </si>
   <si>
     <t>Remove sharps and flats during calibration</t>
+  </si>
+  <si>
+    <t>FILE FORMAT ISSUE. Must figure out how to convert mp3 into ima4 to save CPU space on iOS</t>
   </si>
 </sst>
 </file>
@@ -491,7 +491,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,7 +557,7 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -571,7 +571,7 @@
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -579,7 +579,7 @@
         <v>42598</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -590,13 +590,13 @@
         <v>42598</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -604,7 +604,7 @@
         <v>42598</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -615,7 +615,7 @@
         <v>42599</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
@@ -626,10 +626,10 @@
         <v>42602</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -637,7 +637,7 @@
         <v>42603</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
@@ -648,7 +648,7 @@
         <v>42604</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -659,13 +659,13 @@
         <v>42604</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
         <v>21</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -673,7 +673,7 @@
         <v>42604</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
@@ -684,7 +684,7 @@
         <v>42604</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
@@ -695,7 +695,7 @@
         <v>42604</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
@@ -706,7 +706,7 @@
         <v>42604</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
notes keep their sharp/flat, new button
</commit_message>
<xml_diff>
--- a/scrum.xlsx
+++ b/scrum.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
   <si>
     <t>date</t>
   </si>
@@ -108,6 +108,15 @@
   </si>
   <si>
     <t>FILE FORMAT ISSUE. Must figure out how to convert mp3 into ima4 to save CPU space on iOS</t>
+  </si>
+  <si>
+    <t>Notes stay sharp or flat at calibration</t>
+  </si>
+  <si>
+    <t>New chord - melody + bass chord + up one third</t>
+  </si>
+  <si>
+    <t>not sure if it's right</t>
   </si>
 </sst>
 </file>
@@ -488,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,7 +699,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>42604</v>
       </c>
@@ -701,7 +710,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>42604</v>
       </c>
@@ -710,6 +719,31 @@
       </c>
       <c r="C18" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>42608</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>42608</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new sharps/flats and no added chord
</commit_message>
<xml_diff>
--- a/scrum.xlsx
+++ b/scrum.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
   <si>
     <t>date</t>
   </si>
@@ -117,6 +117,12 @@
   </si>
   <si>
     <t>not sure if it's right</t>
+  </si>
+  <si>
+    <t>think up new UI to enhance chords</t>
+  </si>
+  <si>
+    <t>adjust sharp/flat based on melody note and key</t>
   </si>
 </sst>
 </file>
@@ -497,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,6 +752,28 @@
         <v>29</v>
       </c>
     </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>42610</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>42610</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
manual selection of chords
</commit_message>
<xml_diff>
--- a/scrum.xlsx
+++ b/scrum.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
   <si>
     <t>date</t>
   </si>
@@ -123,6 +123,12 @@
   </si>
   <si>
     <t>adjust sharp/flat based on melody note and key</t>
+  </si>
+  <si>
+    <t>program is coded to allow new audio but loop is still in progress</t>
+  </si>
+  <si>
+    <t>cannot select middle low 3rd or middle low 5th</t>
   </si>
 </sst>
 </file>
@@ -506,7 +512,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,6 +566,9 @@
       <c r="C4" t="s">
         <v>7</v>
       </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -760,7 +769,10 @@
         <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
more rows, improved righttoleft
</commit_message>
<xml_diff>
--- a/scrum.xlsx
+++ b/scrum.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
   <si>
     <t>date</t>
   </si>
@@ -107,9 +107,6 @@
     <t>Remove sharps and flats during calibration</t>
   </si>
   <si>
-    <t>FILE FORMAT ISSUE. Must figure out how to convert mp3 into ima4 to save CPU space on iOS</t>
-  </si>
-  <si>
     <t>Notes stay sharp or flat at calibration</t>
   </si>
   <si>
@@ -129,6 +126,30 @@
   </si>
   <si>
     <t>cannot select middle low 3rd or middle low 5th</t>
+  </si>
+  <si>
+    <t>Remove last column onclick in melody cells</t>
+  </si>
+  <si>
+    <t>Right side key is not written</t>
+  </si>
+  <si>
+    <t>Left to right modulation is not stopping properly</t>
+  </si>
+  <si>
+    <t>Add major and minor key indicator</t>
+  </si>
+  <si>
+    <t>replace lower rows and register</t>
+  </si>
+  <si>
+    <t>Add leading tone rule</t>
+  </si>
+  <si>
+    <t>add 2 octaves</t>
+  </si>
+  <si>
+    <t>works on Chrome</t>
   </si>
 </sst>
 </file>
@@ -509,15 +530,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="63.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -567,7 +588,7 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -592,10 +613,10 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -741,7 +762,7 @@
         <v>42608</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
@@ -752,13 +773,13 @@
         <v>42608</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
         <v>28</v>
-      </c>
-      <c r="C20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -766,13 +787,13 @@
         <v>42610</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -780,10 +801,79 @@
         <v>42610</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>42614</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>42614</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>42614</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>42614</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>42614</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>42619</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>